<commit_message>
added annotations for male/female words
</commit_message>
<xml_diff>
--- a/resources/Lijst_kranten_delpher_10jaar.xlsx
+++ b/resources/Lijst_kranten_delpher_10jaar.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kbeelen/Documents/OtherProjects/KBRiR/KB-RiR/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4898184-6141-5E49-8A1E-E4067795326F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5D24B1-4DEE-B042-84F8-82C22F041A94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -875,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="K131" sqref="K131"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>